<commit_message>
updated App to be able to load data from multiple sites
</commit_message>
<xml_diff>
--- a/data/site_coordinates_UQAM.xlsx
+++ b/data/site_coordinates_UQAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraknox/Code/flux_shiny_plots/ini files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saraknox/Code/RShinyServer/carbonique_RShiny_app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8C7CD4-7D47-B045-82CE-D7D9DD49E445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51C4B2D-1F0E-ED40-B098-0AEF762D97DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" xr2:uid="{CB0BCF3E-B71F-EF4A-9BCC-1E443AF5C85E}"/>
+    <workbookView xWindow="31400" yWindow="2760" windowWidth="25600" windowHeight="14380" xr2:uid="{CB0BCF3E-B71F-EF4A-9BCC-1E443AF5C85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Site</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Standard_Meridian</t>
+  </si>
+  <si>
+    <t>UQAM_2</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B88638-849E-DC4F-84CB-36CB1B1B8DFB}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,6 +461,34 @@
         <v>-72.684443999999999</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>-75</v>
+      </c>
+      <c r="C3">
+        <v>46.531700000000001</v>
+      </c>
+      <c r="D3">
+        <v>-72.6447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-75</v>
+      </c>
+      <c r="C4">
+        <v>46.527971999999998</v>
+      </c>
+      <c r="D4">
+        <v>-72.646249999999995</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>